<commit_message>
changes to handling of kwargs for scatter plots
</commit_message>
<xml_diff>
--- a/Docs/AugerQuant_function_descriptions.xlsx
+++ b/Docs/AugerQuant_function_descriptions.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Functions" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Functions!$A$1:$I$163</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Functions!$A$1:$I$164</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -287,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H106" authorId="0">
+    <comment ref="H107" authorId="0">
       <text>
         <r>
           <rPr>
@@ -300,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G109" authorId="0">
+    <comment ref="G110" authorId="0">
       <text>
         <r>
           <rPr>
@@ -313,7 +313,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H113" authorId="0">
+    <comment ref="H114" authorId="0">
       <text>
         <r>
           <rPr>
@@ -328,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H114" authorId="0">
+    <comment ref="H115" authorId="0">
       <text>
         <r>
           <rPr>
@@ -354,7 +354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H116" authorId="1">
+    <comment ref="H117" authorId="1">
       <text>
         <r>
           <rPr>
@@ -367,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H117" authorId="0">
+    <comment ref="H118" authorId="0">
       <text>
         <r>
           <rPr>
@@ -393,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H139" authorId="0">
+    <comment ref="H140" authorId="0">
       <text>
         <r>
           <rPr>
@@ -406,7 +406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H141" authorId="0">
+    <comment ref="H142" authorId="0">
       <text>
         <r>
           <rPr>
@@ -419,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H146" authorId="0">
+    <comment ref="H147" authorId="0">
       <text>
         <r>
           <rPr>
@@ -437,7 +437,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="337">
   <si>
     <t>Status</t>
   </si>
@@ -1439,6 +1439,15 @@
   </si>
   <si>
     <t>getelemthresholds, parseelem, cloneparamrows</t>
+  </si>
+  <si>
+    <t>get_plotkwargs</t>
+  </si>
+  <si>
+    <t>scattercompplot, others?</t>
+  </si>
+  <si>
+    <t>find and set x and y error columns (if requested by passed kwargs)</t>
   </si>
 </sst>
 </file>
@@ -1825,13 +1834,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C60" sqref="C60"/>
+      <selection pane="bottomRight" activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3123,26 +3132,29 @@
         <v>332</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
-      <c r="A104" t="s">
+    <row r="103" spans="1:8">
+      <c r="A103" t="s">
         <v>37</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B103" t="s">
+        <v>334</v>
+      </c>
+      <c r="C103" t="s">
+        <v>335</v>
+      </c>
+      <c r="H103" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>37</v>
+      </c>
+      <c r="B105" t="s">
         <v>219</v>
       </c>
-      <c r="H104" t="s">
+      <c r="H105" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8">
-      <c r="A106" t="s">
-        <v>37</v>
-      </c>
-      <c r="B106" t="s">
-        <v>270</v>
-      </c>
-      <c r="H106" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3150,10 +3162,10 @@
         <v>37</v>
       </c>
       <c r="B107" t="s">
-        <v>212</v>
+        <v>270</v>
       </c>
       <c r="H107" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -3161,16 +3173,10 @@
         <v>37</v>
       </c>
       <c r="B108" t="s">
-        <v>163</v>
-      </c>
-      <c r="E108" t="s">
-        <v>170</v>
-      </c>
-      <c r="G108" t="s">
-        <v>177</v>
+        <v>212</v>
       </c>
       <c r="H108" t="s">
-        <v>176</v>
+        <v>215</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -3178,10 +3184,16 @@
         <v>37</v>
       </c>
       <c r="B109" t="s">
-        <v>128</v>
+        <v>163</v>
+      </c>
+      <c r="E109" t="s">
+        <v>170</v>
       </c>
       <c r="G109" t="s">
-        <v>208</v>
+        <v>177</v>
+      </c>
+      <c r="H109" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -3189,35 +3201,26 @@
         <v>37</v>
       </c>
       <c r="B110" t="s">
+        <v>128</v>
+      </c>
+      <c r="G110" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" t="s">
+        <v>37</v>
+      </c>
+      <c r="B111" t="s">
         <v>209</v>
       </c>
-      <c r="H110" t="s">
+      <c r="H111" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
-      <c r="B111" s="2" t="s">
+    <row r="112" spans="1:8">
+      <c r="B112" s="2" t="s">
         <v>295</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9">
-      <c r="A113" t="s">
-        <v>37</v>
-      </c>
-      <c r="B113" t="s">
-        <v>15</v>
-      </c>
-      <c r="C113" t="s">
-        <v>181</v>
-      </c>
-      <c r="G113" t="s">
-        <v>14</v>
-      </c>
-      <c r="H113" t="s">
-        <v>178</v>
-      </c>
-      <c r="I113" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -3225,30 +3228,30 @@
         <v>37</v>
       </c>
       <c r="B114" t="s">
+        <v>15</v>
+      </c>
+      <c r="C114" t="s">
+        <v>181</v>
+      </c>
+      <c r="G114" t="s">
+        <v>14</v>
+      </c>
+      <c r="H114" t="s">
+        <v>178</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" t="s">
+        <v>37</v>
+      </c>
+      <c r="B115" t="s">
         <v>207</v>
       </c>
-      <c r="H114" t="s">
+      <c r="H115" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9">
-      <c r="A116" t="s">
-        <v>37</v>
-      </c>
-      <c r="B116" t="s">
-        <v>122</v>
-      </c>
-      <c r="C116" t="s">
-        <v>159</v>
-      </c>
-      <c r="E116" t="s">
-        <v>10</v>
-      </c>
-      <c r="G116" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="H116" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="117" spans="1:9">
@@ -3256,18 +3259,30 @@
         <v>37</v>
       </c>
       <c r="B117" t="s">
+        <v>122</v>
+      </c>
+      <c r="C117" t="s">
+        <v>159</v>
+      </c>
+      <c r="E117" t="s">
+        <v>10</v>
+      </c>
+      <c r="G117" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="H117" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118" t="s">
+        <v>37</v>
+      </c>
+      <c r="B118" t="s">
         <v>17</v>
       </c>
-      <c r="H117" t="s">
+      <c r="H118" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9">
-      <c r="A119" t="s">
-        <v>37</v>
-      </c>
-      <c r="B119" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="120" spans="1:9">
@@ -3275,13 +3290,7 @@
         <v>37</v>
       </c>
       <c r="B120" t="s">
-        <v>105</v>
-      </c>
-      <c r="C120" t="s">
-        <v>120</v>
-      </c>
-      <c r="H120" t="s">
-        <v>106</v>
+        <v>40</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -3289,29 +3298,29 @@
         <v>37</v>
       </c>
       <c r="B121" t="s">
+        <v>105</v>
+      </c>
+      <c r="C121" t="s">
+        <v>120</v>
+      </c>
+      <c r="H121" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122" t="s">
+        <v>37</v>
+      </c>
+      <c r="B122" t="s">
         <v>38</v>
       </c>
-      <c r="H121" t="s">
+      <c r="H122" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
-      <c r="A123" s="1" t="s">
+    <row r="124" spans="1:9">
+      <c r="A124" s="1" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9">
-      <c r="A124" t="s">
-        <v>37</v>
-      </c>
-      <c r="B124" t="s">
-        <v>16</v>
-      </c>
-      <c r="G124" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="H124" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -3319,34 +3328,36 @@
         <v>37</v>
       </c>
       <c r="B125" t="s">
-        <v>107</v>
-      </c>
-      <c r="E125" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G125" s="4" t="s">
         <v>160</v>
       </c>
       <c r="H125" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126" t="s">
+        <v>37</v>
+      </c>
+      <c r="B126" t="s">
+        <v>107</v>
+      </c>
+      <c r="E126" t="s">
+        <v>10</v>
+      </c>
+      <c r="G126" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="H126" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
-      <c r="A127" s="1"/>
-      <c r="B127" t="s">
+    <row r="128" spans="1:9">
+      <c r="A128" s="1"/>
+      <c r="B128" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9">
-      <c r="A128" t="s">
-        <v>37</v>
-      </c>
-      <c r="B128" t="s">
-        <v>161</v>
-      </c>
-      <c r="G128" s="4"/>
-      <c r="H128" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -3354,13 +3365,11 @@
         <v>37</v>
       </c>
       <c r="B129" t="s">
-        <v>5</v>
-      </c>
-      <c r="G129" t="s">
-        <v>14</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="G129" s="4"/>
       <c r="H129" t="s">
-        <v>4</v>
+        <v>162</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -3368,13 +3377,13 @@
         <v>37</v>
       </c>
       <c r="B130" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G130" t="s">
         <v>14</v>
       </c>
       <c r="H130" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -3382,13 +3391,13 @@
         <v>37</v>
       </c>
       <c r="B131" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G131" t="s">
         <v>14</v>
       </c>
       <c r="H131" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -3396,13 +3405,13 @@
         <v>37</v>
       </c>
       <c r="B132" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G132" t="s">
         <v>14</v>
       </c>
       <c r="H132" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -3410,13 +3419,13 @@
         <v>37</v>
       </c>
       <c r="B133" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G133" t="s">
         <v>14</v>
       </c>
       <c r="H133" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -3424,16 +3433,13 @@
         <v>37</v>
       </c>
       <c r="B134" t="s">
-        <v>164</v>
-      </c>
-      <c r="C134" t="s">
-        <v>167</v>
-      </c>
-      <c r="D134" t="s">
-        <v>168</v>
+        <v>12</v>
+      </c>
+      <c r="G134" t="s">
+        <v>14</v>
       </c>
       <c r="H134" t="s">
-        <v>165</v>
+        <v>13</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -3441,69 +3447,66 @@
         <v>37</v>
       </c>
       <c r="B135" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C135" t="s">
         <v>167</v>
       </c>
       <c r="D135" t="s">
+        <v>168</v>
+      </c>
+      <c r="H135" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" t="s">
+        <v>37</v>
+      </c>
+      <c r="B136" t="s">
+        <v>161</v>
+      </c>
+      <c r="C136" t="s">
+        <v>167</v>
+      </c>
+      <c r="D136" t="s">
         <v>169</v>
       </c>
-      <c r="H135" t="s">
+      <c r="H136" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
-      <c r="B137" s="2" t="s">
+    <row r="138" spans="1:8">
+      <c r="B138" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="H137" t="s">
+      <c r="H138" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
-      <c r="B138" t="s">
+    <row r="139" spans="1:8">
+      <c r="B139" t="s">
         <v>197</v>
       </c>
-      <c r="H138" t="s">
+      <c r="H139" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
-      <c r="A139" t="s">
+    <row r="140" spans="1:8">
+      <c r="A140" t="s">
         <v>84</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B140" t="s">
         <v>90</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C140" t="s">
         <v>89</v>
       </c>
-      <c r="G139" t="s">
+      <c r="G140" t="s">
         <v>100</v>
       </c>
-      <c r="H139" t="s">
+      <c r="H140" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8">
-      <c r="A141" t="s">
-        <v>101</v>
-      </c>
-      <c r="B141" t="s">
-        <v>320</v>
-      </c>
-      <c r="C141" t="s">
-        <v>120</v>
-      </c>
-      <c r="D141" t="s">
-        <v>317</v>
-      </c>
-      <c r="G141" t="s">
-        <v>100</v>
-      </c>
-      <c r="H141" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -3511,38 +3514,47 @@
         <v>101</v>
       </c>
       <c r="B142" t="s">
-        <v>264</v>
+        <v>320</v>
+      </c>
+      <c r="C142" t="s">
+        <v>120</v>
+      </c>
+      <c r="D142" t="s">
+        <v>317</v>
+      </c>
+      <c r="G142" t="s">
+        <v>100</v>
       </c>
       <c r="H142" t="s">
-        <v>265</v>
+        <v>316</v>
       </c>
     </row>
     <row r="143" spans="1:8">
       <c r="A143" t="s">
         <v>101</v>
       </c>
-      <c r="B143" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C143" t="s">
+      <c r="B143" t="s">
         <v>264</v>
       </c>
-      <c r="G143" t="s">
-        <v>268</v>
-      </c>
       <c r="H143" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="144" spans="1:8">
       <c r="A144" t="s">
         <v>101</v>
       </c>
-      <c r="B144" t="s">
-        <v>102</v>
+      <c r="B144" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C144" t="s">
+        <v>264</v>
+      </c>
+      <c r="G144" t="s">
+        <v>268</v>
       </c>
       <c r="H144" t="s">
-        <v>103</v>
+        <v>267</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -3550,10 +3562,10 @@
         <v>101</v>
       </c>
       <c r="B145" t="s">
-        <v>182</v>
+        <v>102</v>
       </c>
       <c r="H145" t="s">
-        <v>183</v>
+        <v>103</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -3561,10 +3573,10 @@
         <v>101</v>
       </c>
       <c r="B146" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H146" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -3572,13 +3584,10 @@
         <v>101</v>
       </c>
       <c r="B147" t="s">
-        <v>195</v>
-      </c>
-      <c r="G147" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="H147" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -3586,10 +3595,13 @@
         <v>101</v>
       </c>
       <c r="B148" t="s">
-        <v>199</v>
+        <v>195</v>
+      </c>
+      <c r="G148" t="s">
+        <v>196</v>
       </c>
       <c r="H148" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -3597,10 +3609,10 @@
         <v>101</v>
       </c>
       <c r="B149" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="H149" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -3608,10 +3620,10 @@
         <v>101</v>
       </c>
       <c r="B150" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H150" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -3619,10 +3631,10 @@
         <v>101</v>
       </c>
       <c r="B151" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="H151" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -3630,10 +3642,10 @@
         <v>101</v>
       </c>
       <c r="B152" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="H152" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -3641,78 +3653,89 @@
         <v>101</v>
       </c>
       <c r="B153" t="s">
+        <v>231</v>
+      </c>
+      <c r="H153" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9">
+      <c r="A154" t="s">
+        <v>101</v>
+      </c>
+      <c r="B154" t="s">
         <v>321</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C154" t="s">
         <v>120</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D154" t="s">
         <v>322</v>
       </c>
-      <c r="H153" t="s">
+      <c r="H154" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
-      <c r="A155" t="s">
+    <row r="156" spans="1:9">
+      <c r="A156" t="s">
         <v>84</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B156" t="s">
         <v>119</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C156" t="s">
         <v>114</v>
       </c>
-      <c r="F155" t="s">
+      <c r="F156" t="s">
         <v>116</v>
       </c>
-      <c r="I155" s="2"/>
-    </row>
-    <row r="156" spans="1:9">
       <c r="I156" s="2"/>
     </row>
     <row r="157" spans="1:9">
-      <c r="A157" t="s">
+      <c r="I157" s="2"/>
+    </row>
+    <row r="158" spans="1:9">
+      <c r="A158" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
-      <c r="B158" t="s">
+    <row r="159" spans="1:9">
+      <c r="B159" t="s">
         <v>143</v>
       </c>
-      <c r="G158" t="s">
+      <c r="G159" t="s">
         <v>145</v>
       </c>
-      <c r="H158" t="s">
+      <c r="H159" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
-      <c r="A160" t="s">
+    <row r="161" spans="1:9">
+      <c r="A161" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="161" spans="2:9">
-      <c r="B161" t="s">
+    <row r="162" spans="1:9">
+      <c r="B162" t="s">
         <v>148</v>
       </c>
-      <c r="H161" t="s">
+      <c r="H162" t="s">
         <v>149</v>
       </c>
-      <c r="I161" t="s">
+      <c r="I162" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="162" spans="2:9">
-      <c r="B162" t="s">
+    <row r="163" spans="1:9">
+      <c r="B163" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="163" spans="2:9">
-      <c r="B163" t="s">
+    <row r="164" spans="1:9">
+      <c r="B164" t="s">
         <v>152</v>
       </c>
-      <c r="H163" t="s">
+      <c r="H164" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added tkinter function for selecting elements
</commit_message>
<xml_diff>
--- a/Docs/AugerQuant_function_descriptions.xlsx
+++ b/Docs/AugerQuant_function_descriptions.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Functions" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Functions!$A$1:$I$164</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Functions!$A$1:$I$165</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -406,7 +406,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="H142" authorId="0">
+    <comment ref="D142" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lines only available if specified in AESquantparams</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H143" authorId="0">
       <text>
         <r>
           <rPr>
@@ -419,7 +432,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H147" authorId="0">
+    <comment ref="H148" authorId="0">
       <text>
         <r>
           <rPr>
@@ -437,7 +450,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="340">
   <si>
     <t>Status</t>
   </si>
@@ -1448,6 +1461,15 @@
   </si>
   <si>
     <t>find and set x and y error columns (if requested by passed kwargs)</t>
+  </si>
+  <si>
+    <t>getelemsGUI</t>
+  </si>
+  <si>
+    <t>interactively choose elements for quant or plots</t>
+  </si>
+  <si>
+    <t>AESquantparams</t>
   </si>
 </sst>
 </file>
@@ -1834,13 +1856,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I164"/>
+  <dimension ref="A1:I165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H105" sqref="H105"/>
+      <selection pane="bottomRight" activeCell="D145" sqref="D145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3514,19 +3536,13 @@
         <v>101</v>
       </c>
       <c r="B142" t="s">
-        <v>320</v>
-      </c>
-      <c r="C142" t="s">
-        <v>120</v>
+        <v>337</v>
       </c>
       <c r="D142" t="s">
-        <v>317</v>
-      </c>
-      <c r="G142" t="s">
-        <v>100</v>
+        <v>339</v>
       </c>
       <c r="H142" t="s">
-        <v>316</v>
+        <v>338</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -3534,38 +3550,47 @@
         <v>101</v>
       </c>
       <c r="B143" t="s">
-        <v>264</v>
+        <v>320</v>
+      </c>
+      <c r="C143" t="s">
+        <v>120</v>
+      </c>
+      <c r="D143" t="s">
+        <v>317</v>
+      </c>
+      <c r="G143" t="s">
+        <v>100</v>
       </c>
       <c r="H143" t="s">
-        <v>265</v>
+        <v>316</v>
       </c>
     </row>
     <row r="144" spans="1:8">
       <c r="A144" t="s">
         <v>101</v>
       </c>
-      <c r="B144" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C144" t="s">
+      <c r="B144" t="s">
         <v>264</v>
       </c>
-      <c r="G144" t="s">
-        <v>268</v>
-      </c>
       <c r="H144" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="145" spans="1:9">
       <c r="A145" t="s">
         <v>101</v>
       </c>
-      <c r="B145" t="s">
-        <v>102</v>
+      <c r="B145" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C145" t="s">
+        <v>264</v>
+      </c>
+      <c r="G145" t="s">
+        <v>268</v>
       </c>
       <c r="H145" t="s">
-        <v>103</v>
+        <v>267</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -3573,10 +3598,10 @@
         <v>101</v>
       </c>
       <c r="B146" t="s">
-        <v>182</v>
+        <v>102</v>
       </c>
       <c r="H146" t="s">
-        <v>183</v>
+        <v>103</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -3584,10 +3609,10 @@
         <v>101</v>
       </c>
       <c r="B147" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H147" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -3595,13 +3620,10 @@
         <v>101</v>
       </c>
       <c r="B148" t="s">
-        <v>195</v>
-      </c>
-      <c r="G148" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="H148" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -3609,10 +3631,13 @@
         <v>101</v>
       </c>
       <c r="B149" t="s">
-        <v>199</v>
+        <v>195</v>
+      </c>
+      <c r="G149" t="s">
+        <v>196</v>
       </c>
       <c r="H149" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -3620,10 +3645,10 @@
         <v>101</v>
       </c>
       <c r="B150" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="H150" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -3631,10 +3656,10 @@
         <v>101</v>
       </c>
       <c r="B151" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H151" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -3642,10 +3667,10 @@
         <v>101</v>
       </c>
       <c r="B152" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="H152" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -3653,10 +3678,10 @@
         <v>101</v>
       </c>
       <c r="B153" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="H153" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -3664,78 +3689,89 @@
         <v>101</v>
       </c>
       <c r="B154" t="s">
+        <v>231</v>
+      </c>
+      <c r="H154" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
+      <c r="A155" t="s">
+        <v>101</v>
+      </c>
+      <c r="B155" t="s">
         <v>321</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C155" t="s">
         <v>120</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D155" t="s">
         <v>322</v>
       </c>
-      <c r="H154" t="s">
+      <c r="H155" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
-      <c r="A156" t="s">
+    <row r="157" spans="1:9">
+      <c r="A157" t="s">
         <v>84</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B157" t="s">
         <v>119</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C157" t="s">
         <v>114</v>
       </c>
-      <c r="F156" t="s">
+      <c r="F157" t="s">
         <v>116</v>
       </c>
-      <c r="I156" s="2"/>
-    </row>
-    <row r="157" spans="1:9">
       <c r="I157" s="2"/>
     </row>
     <row r="158" spans="1:9">
-      <c r="A158" t="s">
+      <c r="I158" s="2"/>
+    </row>
+    <row r="159" spans="1:9">
+      <c r="A159" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="159" spans="1:9">
-      <c r="B159" t="s">
+    <row r="160" spans="1:9">
+      <c r="B160" t="s">
         <v>143</v>
       </c>
-      <c r="G159" t="s">
+      <c r="G160" t="s">
         <v>145</v>
       </c>
-      <c r="H159" t="s">
+      <c r="H160" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
-      <c r="A161" t="s">
+    <row r="162" spans="1:9">
+      <c r="A162" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9">
-      <c r="B162" t="s">
-        <v>148</v>
-      </c>
-      <c r="H162" t="s">
-        <v>149</v>
-      </c>
-      <c r="I162" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="B163" t="s">
-        <v>151</v>
+        <v>148</v>
+      </c>
+      <c r="H163" t="s">
+        <v>149</v>
+      </c>
+      <c r="I163" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="B164" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
+      <c r="B165" t="s">
         <v>152</v>
       </c>
-      <c r="H164" t="s">
+      <c r="H165" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>